<commit_message>
Create French satisfaction files and update zufriedenheit files
</commit_message>
<xml_diff>
--- a/einf_r/zufriedenheit.xlsx
+++ b/einf_r/zufriedenheit.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28108"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10811"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrew/Teaching/425464-FS2017-intro-to-R/book/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/borismayer/Documents/R_Repos/data/einf_r/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE096B23-E53F-5F4B-B0B8-14C3C264064E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17600" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17600" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="zufriedenheit" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -29,37 +30,37 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="9">
   <si>
-    <t>Vpn</t>
-  </si>
-  <si>
     <t>messzeitpunkt</t>
   </si>
   <si>
-    <t>rating</t>
-  </si>
-  <si>
-    <t>VP_1</t>
-  </si>
-  <si>
     <t>t1</t>
   </si>
   <si>
-    <t>VP_2</t>
-  </si>
-  <si>
-    <t>VP_3</t>
-  </si>
-  <si>
-    <t>VP_4</t>
-  </si>
-  <si>
     <t>t2</t>
+  </si>
+  <si>
+    <t>vpn</t>
+  </si>
+  <si>
+    <t>zufriedenheit</t>
+  </si>
+  <si>
+    <t>vp_1</t>
+  </si>
+  <si>
+    <t>vp_2</t>
+  </si>
+  <si>
+    <t>vp_3</t>
+  </si>
+  <si>
+    <t>vp_4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -93,13 +94,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -367,30 +371,32 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C2">
         <v>64.290000000000006</v>
@@ -398,10 +404,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C3">
         <v>65.06</v>
@@ -409,10 +415,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C4">
         <v>54.25</v>
@@ -420,10 +426,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C5">
         <v>54.53</v>
@@ -431,10 +437,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="C6">
         <v>67.239999999999995</v>
@@ -442,10 +448,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="C7">
         <v>75.64</v>
@@ -453,10 +459,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="C8">
         <v>84.59</v>
@@ -464,10 +470,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="C9">
         <v>73.900000000000006</v>

</xml_diff>